<commit_message>
novo modelo, bd revisado
</commit_message>
<xml_diff>
--- a/filtros/objeto.xlsx
+++ b/filtros/objeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CAD-TI\SERVIDORES\Augusto\workspace\classificador_tic\filtros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE645D-306B-4EBD-8196-AECB973C754F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36AF621-C9BC-4075-A699-443D5C9DC1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>Telecom</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>tot(?:em|en)s?</t>
+  </si>
+  <si>
+    <t>arduino</t>
   </si>
 </sst>
 </file>
@@ -699,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L108" sqref="L108"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,6 +1315,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adicionado mais modelos treinados com base revisada
</commit_message>
<xml_diff>
--- a/filtros/objeto.xlsx
+++ b/filtros/objeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CAD-TI\SERVIDORES\Augusto\workspace\classificador_tic\filtros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53029D08-A848-4521-B915-D3C6875B2EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C3257-1E07-4D09-80BE-7DC0D7818334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
   <si>
     <t>Telecom</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>ponto de funcao</t>
+  </si>
+  <si>
+    <t>sistema</t>
+  </si>
+  <si>
+    <t>anti.{0,1}virus</t>
   </si>
 </sst>
 </file>
@@ -711,11 +717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,6 +1350,16 @@
         <v>110</v>
       </c>
     </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adicionado mais termos ao filtro_ti
</commit_message>
<xml_diff>
--- a/filtros/objeto.xlsx
+++ b/filtros/objeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CAD-TI\SERVIDORES\Augusto\workspace\classificador_tic\filtros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C3257-1E07-4D09-80BE-7DC0D7818334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99AF383-D7DD-4581-B5C4-8C504E7062F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26295" yWindow="1665" windowWidth="25500" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
   <si>
     <t>Telecom</t>
   </si>
@@ -212,9 +212,6 @@
     <t>licenca.{0,10}perpetua</t>
   </si>
   <si>
-    <t>certificado.{0,10}digita\S{1,2}</t>
-  </si>
-  <si>
     <t>nvme</t>
   </si>
   <si>
@@ -375,6 +372,18 @@
   </si>
   <si>
     <t>anti.{0,1}virus</t>
+  </si>
+  <si>
+    <t>ssl</t>
+  </si>
+  <si>
+    <t>certifica.{0,10}digita\S{1,2}</t>
+  </si>
+  <si>
+    <t>plataforma digital</t>
+  </si>
+  <si>
+    <t>token</t>
   </si>
 </sst>
 </file>
@@ -717,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +771,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -778,7 +787,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +807,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -833,7 +842,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,7 +880,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +895,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -917,7 +926,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -953,7 +962,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +982,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,7 +1038,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
         <v>30</v>
@@ -1037,7 +1046,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1052,7 +1061,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
@@ -1081,7 +1090,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1120,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,12 +1130,12 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
@@ -1134,7 +1143,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
         <v>30</v>
@@ -1142,7 +1151,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
         <v>30</v>
@@ -1150,42 +1159,42 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
         <v>30</v>
@@ -1193,17 +1202,17 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
         <v>30</v>
@@ -1211,17 +1220,17 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
         <v>30</v>
@@ -1229,12 +1238,12 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
         <v>30</v>
@@ -1242,27 +1251,27 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>30</v>
@@ -1270,7 +1279,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>30</v>
@@ -1278,22 +1287,22 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B99" t="s">
         <v>30</v>
@@ -1301,12 +1310,12 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>30</v>
@@ -1314,17 +1323,17 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
         <v>30</v>
@@ -1332,32 +1341,50 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>112</v>
+      </c>
+      <c r="B111" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>